<commit_message>
Updated scripts and output validation files
</commit_message>
<xml_diff>
--- a/CDE_ID_detective_revamp/in/HDP00980_iHOPEAim1_DataDictionary.xlsx
+++ b/CDE_ID_detective_revamp/in/HDP00980_iHOPEAim1_DataDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmaefos\Code Stuffs\CDE_detective\CDE_ID_detective_revamp\in\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{891890A6-9CFF-4F4C-AEE2-9B0516FC6634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0CBE6F7-E92C-4AC7-B7D9-0C0BC1CD6C1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38505" yWindow="6465" windowWidth="19410" windowHeight="20985" xr2:uid="{A4D67A7F-894F-4EEF-A0AA-6B28BA297F7F}"/>
+    <workbookView xWindow="-29535" yWindow="8025" windowWidth="21495" windowHeight="18660" xr2:uid="{A4D67A7F-894F-4EEF-A0AA-6B28BA297F7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1400,13 +1400,16 @@
   <dimension ref="A1:R53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="15.73046875" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.06640625" style="1"/>
+    <col min="2" max="4" width="9.06640625" style="1"/>
+    <col min="5" max="5" width="29.06640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="40.9296875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.45">

</xml_diff>